<commit_message>
Pre plan team draft updates with edits included
</commit_message>
<xml_diff>
--- a/examples/smbkc_18/doc/Table_for_SS3.xlsx
+++ b/examples/smbkc_18/doc/Table_for_SS3.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jim/_mymods/seacode/gmacs/examples/smbkc_18/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{6568B315-0A11-4F42-BAF0-C8083361FD1F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{192DB394-8770-704F-92A9-D548B793FC23}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="460" windowWidth="33600" windowHeight="18440" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="3" r:id="rId1"/>
@@ -838,10 +838,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="19">
     <font>
@@ -1332,7 +1332,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
@@ -3027,6 +3027,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="1433067744"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -4194,10 +4195,10 @@
 </file>
 
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="144" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="149" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4208,7 +4209,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8669514" cy="6279444"/>
+    <xdr:ext cx="8676913" cy="6281812"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -4574,11 +4575,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AF94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="150" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="S44" sqref="S44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4676,6 +4677,10 @@
         <f>F4/D4</f>
         <v>0.20380768893197876</v>
       </c>
+      <c r="J4">
+        <f>RANK(H4,H4:H44)</f>
+        <v>9</v>
+      </c>
       <c r="K4">
         <v>9381.6943580000006</v>
       </c>
@@ -4702,7 +4707,7 @@
         <v>0.39400000000000002</v>
       </c>
       <c r="W4" s="2">
-        <f t="shared" ref="W4:W44" si="1">U4/$U$47</f>
+        <f t="shared" ref="W4:W43" si="1">U4/$U$47</f>
         <v>1.2062721293231626</v>
       </c>
       <c r="Z4">
@@ -7936,7 +7941,7 @@
       <c r="O52" s="4"/>
       <c r="P52" s="4"/>
       <c r="S52" s="2">
-        <f t="shared" ref="S52:S92" si="5">B52/B$94</f>
+        <f t="shared" ref="S52:S91" si="5">B52/B$94</f>
         <v>2.1242976212773934</v>
       </c>
       <c r="T52" s="2">
@@ -10557,7 +10562,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AN401"/>
   <sheetViews>
     <sheetView topLeftCell="A245" zoomScale="215" workbookViewId="0">

</xml_diff>